<commit_message>
Adição de tela inserir passageiro em voo
</commit_message>
<xml_diff>
--- a/BD.xlsx
+++ b/BD.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" tabRatio="600" firstSheet="0" activeTab="2" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="Voos" sheetId="1" state="visible" r:id="rId1"/>
@@ -359,8 +359,8 @@
   </sheetPr>
   <dimension ref="A1:F4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
@@ -447,7 +447,7 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>São Paulo</t>
+          <t>Sao Paulo</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
@@ -503,10 +503,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:F4"/>
+      <selection activeCell="A8" sqref="A8:XFD8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
@@ -585,6 +585,131 @@
       <c r="E3" t="inlineStr">
         <is>
           <t>ana@gmail.com</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Anthony</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>00055522200</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>87545454211</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>dasd@gmail.com</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>4</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>João</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>55566988544</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>874545545544</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>asdasd@gmail.com</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>5</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Marcia</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>588545456564</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>87784546465</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>saddas@gmail.com</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>6</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Joana</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>5154565456</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>8756542123</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>asdas@gmail.com</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>8</v>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>André</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>154554546546565</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>8778455456465</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>asdasd@gmail.com</t>
         </is>
       </c>
     </row>
@@ -601,8 +726,8 @@
   </sheetPr>
   <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A2:R3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
@@ -642,15 +767,17 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="C2" t="n">
-        <v>20</v>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>21</t>
+        </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>economica</t>
+          <t>Executiva</t>
         </is>
       </c>
       <c r="E2" t="n">

</xml_diff>